<commit_message>
Se adiciono la capa de presentacion LOGIN
</commit_message>
<xml_diff>
--- a/Nomina_trabajos finales.xlsx
+++ b/Nomina_trabajos finales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogerruizescobar/Documents/UDABOL/UDABOL_202202/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F31C16-4BFF-444E-8579-F8F058264961}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7173210-7BDA-974E-8516-E05730B2FD9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="461">
   <si>
     <t>Leonardo</t>
   </si>
@@ -2583,7 +2583,7 @@
   <dimension ref="A1:R151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P58" sqref="P58"/>
+      <selection activeCell="P53" sqref="P53:P57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4897,7 +4897,7 @@
       <c r="Q47" s="8"/>
       <c r="R47" s="8"/>
     </row>
-    <row r="48" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="18">
         <v>38</v>
       </c>
@@ -4950,7 +4950,7 @@
       <c r="Q48" s="8"/>
       <c r="R48" s="8"/>
     </row>
-    <row r="49" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="18">
         <v>48</v>
       </c>
@@ -4997,7 +4997,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="P49" s="8"/>
+      <c r="P49" s="8" t="s">
+        <v>458</v>
+      </c>
       <c r="Q49" s="8"/>
       <c r="R49" s="8"/>
     </row>
@@ -5054,7 +5056,7 @@
       <c r="Q50" s="8"/>
       <c r="R50" s="8"/>
     </row>
-    <row r="51" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="18">
         <v>18</v>
       </c>
@@ -5101,11 +5103,13 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="P51" s="8"/>
+      <c r="P51" s="8" t="s">
+        <v>458</v>
+      </c>
       <c r="Q51" s="8"/>
       <c r="R51" s="8"/>
     </row>
-    <row r="52" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="18">
         <v>28</v>
       </c>
@@ -5152,7 +5156,9 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="P52" s="8"/>
+      <c r="P52" s="8" t="s">
+        <v>458</v>
+      </c>
       <c r="Q52" s="8"/>
       <c r="R52" s="8"/>
     </row>
@@ -5256,7 +5262,9 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="P54" s="8"/>
+      <c r="P54" s="8" t="s">
+        <v>459</v>
+      </c>
       <c r="Q54" s="8"/>
       <c r="R54" s="8"/>
     </row>
@@ -5307,7 +5315,9 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="P55" s="8"/>
+      <c r="P55" s="8" t="s">
+        <v>459</v>
+      </c>
       <c r="Q55" s="8"/>
       <c r="R55" s="8"/>
     </row>
@@ -5358,7 +5368,9 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="P56" s="8"/>
+      <c r="P56" s="8" t="s">
+        <v>459</v>
+      </c>
       <c r="Q56" s="8"/>
       <c r="R56" s="8"/>
     </row>
@@ -5409,7 +5421,9 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="P57" s="8"/>
+      <c r="P57" s="8" t="s">
+        <v>459</v>
+      </c>
       <c r="Q57" s="8"/>
       <c r="R57" s="8"/>
     </row>
@@ -7204,6 +7218,7 @@
     <filterColumn colId="15">
       <filters>
         <filter val="Mono"/>
+        <filter val="Presentacion Menu Operaciones con mensajes"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Actualizacion de la lista de trabajos
</commit_message>
<xml_diff>
--- a/Nomina_trabajos finales.xlsx
+++ b/Nomina_trabajos finales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogerruizescobar/Documents/UDABOL/UDABOL_202202/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7173210-7BDA-974E-8516-E05730B2FD9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3ACFC9-92A5-6D47-87FB-63C869CCF138}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="471">
   <si>
     <t>Leonardo</t>
   </si>
@@ -1412,6 +1412,36 @@
   </si>
   <si>
     <t>Mono</t>
+  </si>
+  <si>
+    <t>insert_delete_PgSql</t>
+  </si>
+  <si>
+    <t>Rama</t>
+  </si>
+  <si>
+    <t>modelo</t>
+  </si>
+  <si>
+    <t>negocio1</t>
+  </si>
+  <si>
+    <t>negocio2</t>
+  </si>
+  <si>
+    <t>negocio3</t>
+  </si>
+  <si>
+    <t>negocio4</t>
+  </si>
+  <si>
+    <t>negocio5</t>
+  </si>
+  <si>
+    <t>negocio6</t>
+  </si>
+  <si>
+    <t>presentacion_mensaje</t>
   </si>
 </sst>
 </file>
@@ -1495,12 +1525,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1531,7 +1567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1581,6 +1617,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2579,11 +2626,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:R151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P53" sqref="P53:P57"/>
+    <sheetView tabSelected="1" topLeftCell="L40" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q51" sqref="Q51:Q52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2600,7 +2646,10 @@
     <col min="11" max="11" width="37.1640625" customWidth="1"/>
     <col min="12" max="12" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="18" width="13.5" customWidth="1"/>
+    <col min="14" max="15" width="13.5" customWidth="1"/>
+    <col min="16" max="16" width="39" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17" customWidth="1"/>
+    <col min="18" max="18" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2646,10 +2695,12 @@
         <v>450</v>
       </c>
       <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
+      <c r="Q1" s="8" t="s">
+        <v>462</v>
+      </c>
       <c r="R1" s="8"/>
     </row>
-    <row r="2" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
         <v>20</v>
       </c>
@@ -2702,7 +2753,7 @@
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
     </row>
-    <row r="3" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="18">
         <v>10</v>
       </c>
@@ -2749,11 +2800,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P3" s="8"/>
+      <c r="P3" s="8" t="s">
+        <v>455</v>
+      </c>
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
     </row>
-    <row r="4" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
         <v>50</v>
       </c>
@@ -2798,11 +2851,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P4" s="8"/>
+      <c r="P4" s="8" t="s">
+        <v>455</v>
+      </c>
       <c r="Q4" s="8"/>
       <c r="R4" s="8"/>
     </row>
-    <row r="5" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>40</v>
       </c>
@@ -2847,11 +2902,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P5" s="8"/>
+      <c r="P5" s="8" t="s">
+        <v>455</v>
+      </c>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
     </row>
-    <row r="6" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>30</v>
       </c>
@@ -2898,11 +2955,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P6" s="8"/>
+      <c r="P6" s="8" t="s">
+        <v>455</v>
+      </c>
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
     </row>
-    <row r="7" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>11</v>
       </c>
@@ -2949,11 +3008,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="P7" s="8"/>
+      <c r="P7" s="8" t="s">
+        <v>455</v>
+      </c>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
     </row>
-    <row r="8" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>51</v>
       </c>
@@ -3003,10 +3064,12 @@
       <c r="P8" s="8" t="s">
         <v>456</v>
       </c>
-      <c r="Q8" s="8"/>
+      <c r="Q8" s="8" t="s">
+        <v>461</v>
+      </c>
       <c r="R8" s="8"/>
     </row>
-    <row r="9" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>41</v>
       </c>
@@ -3053,11 +3116,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
+      <c r="P9" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>461</v>
+      </c>
       <c r="R9" s="8"/>
     </row>
-    <row r="10" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
         <v>31</v>
       </c>
@@ -3104,11 +3171,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
+      <c r="P10" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>461</v>
+      </c>
       <c r="R10" s="8"/>
     </row>
-    <row r="11" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
         <v>21</v>
       </c>
@@ -3155,11 +3226,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
+      <c r="P11" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>461</v>
+      </c>
       <c r="R11" s="8"/>
     </row>
-    <row r="12" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
         <v>1</v>
       </c>
@@ -3206,11 +3281,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
+      <c r="P12" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="Q12" s="8" t="s">
+        <v>461</v>
+      </c>
       <c r="R12" s="8"/>
     </row>
-    <row r="13" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>32</v>
       </c>
@@ -3260,10 +3339,12 @@
       <c r="P13" s="8" t="s">
         <v>451</v>
       </c>
-      <c r="Q13" s="8"/>
+      <c r="Q13" s="8" t="s">
+        <v>464</v>
+      </c>
       <c r="R13" s="8"/>
     </row>
-    <row r="14" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>42</v>
       </c>
@@ -3308,11 +3389,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
+      <c r="P14" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>465</v>
+      </c>
       <c r="R14" s="8"/>
     </row>
-    <row r="15" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>2</v>
       </c>
@@ -3359,11 +3444,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
+      <c r="P15" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q15" s="8" t="s">
+        <v>466</v>
+      </c>
       <c r="R15" s="8"/>
     </row>
-    <row r="16" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>22</v>
       </c>
@@ -3410,11 +3499,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
+      <c r="P16" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q16" s="8" t="s">
+        <v>467</v>
+      </c>
       <c r="R16" s="8"/>
     </row>
-    <row r="17" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <v>12</v>
       </c>
@@ -3461,11 +3554,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="8"/>
+      <c r="P17" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q17" s="8" t="s">
+        <v>468</v>
+      </c>
       <c r="R17" s="8"/>
     </row>
-    <row r="18" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
         <v>52</v>
       </c>
@@ -3490,297 +3587,323 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
+      <c r="P18" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="Q18" s="8" t="s">
+        <v>469</v>
+      </c>
       <c r="R18" s="8"/>
     </row>
-    <row r="19" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="18">
+    <row r="19" spans="1:18" s="23" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="19">
         <v>33</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="20">
         <v>44816.9083217593</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="21" t="s">
         <v>324</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="21" t="s">
         <v>325</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="21" t="s">
         <v>326</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="21" t="s">
         <v>327</v>
       </c>
-      <c r="I19" s="10" t="s">
+      <c r="I19" s="21" t="s">
         <v>328</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="J19" s="21" t="s">
         <v>329</v>
       </c>
-      <c r="K19" s="10" t="s">
+      <c r="K19" s="21" t="s">
         <v>323</v>
       </c>
-      <c r="L19" s="10" t="s">
+      <c r="L19" s="21" t="s">
         <v>330</v>
       </c>
-      <c r="M19" s="10" t="s">
+      <c r="M19" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="N19" s="10">
+      <c r="N19" s="21">
         <v>33</v>
       </c>
-      <c r="O19" s="10">
+      <c r="O19" s="21">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="P19" s="8" t="s">
+      <c r="P19" s="22" t="s">
         <v>452</v>
       </c>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-    </row>
-    <row r="20" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="18">
+      <c r="Q19" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="R19" s="22"/>
+    </row>
+    <row r="20" spans="1:18" s="23" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="19">
         <v>43</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="20">
         <v>44818.452256944402</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="21" t="s">
         <v>384</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="21" t="s">
         <v>385</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="21" t="s">
         <v>387</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="21" t="s">
         <v>384</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="21" t="s">
         <v>388</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="21" t="s">
         <v>389</v>
       </c>
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="21" t="s">
         <v>390</v>
       </c>
-      <c r="K20" s="10" t="s">
+      <c r="K20" s="21" t="s">
         <v>384</v>
       </c>
-      <c r="L20" s="10" t="s">
+      <c r="L20" s="21" t="s">
         <v>391</v>
       </c>
-      <c r="M20" s="10" t="s">
+      <c r="M20" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="N20" s="10">
+      <c r="N20" s="21">
         <v>43</v>
       </c>
-      <c r="O20" s="10">
+      <c r="O20" s="21">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-    </row>
-    <row r="21" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="18">
+      <c r="P20" s="22" t="s">
+        <v>452</v>
+      </c>
+      <c r="Q20" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="R20" s="22"/>
+    </row>
+    <row r="21" spans="1:18" s="23" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="19">
         <v>23</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="20">
         <v>44816.904606481497</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="21" t="s">
         <v>258</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="21" t="s">
         <v>261</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="J21" s="10" t="s">
+      <c r="J21" s="21" t="s">
         <v>263</v>
       </c>
-      <c r="K21" s="10" t="s">
+      <c r="K21" s="21" t="s">
         <v>257</v>
       </c>
-      <c r="L21" s="10" t="s">
+      <c r="L21" s="21" t="s">
         <v>260</v>
       </c>
-      <c r="M21" s="10" t="s">
+      <c r="M21" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="N21" s="10">
+      <c r="N21" s="21">
         <v>23</v>
       </c>
-      <c r="O21" s="10">
+      <c r="O21" s="21">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-    </row>
-    <row r="22" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="18">
+      <c r="P21" s="22" t="s">
+        <v>452</v>
+      </c>
+      <c r="Q21" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="R21" s="22"/>
+    </row>
+    <row r="22" spans="1:18" s="23" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="19">
         <v>13</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="20">
         <v>44816.902129629598</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="H22" s="10" t="s">
+      <c r="H22" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="I22" s="10" t="s">
+      <c r="I22" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="J22" s="10" t="s">
+      <c r="J22" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="K22" s="10" t="s">
+      <c r="K22" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="L22" s="10" t="s">
+      <c r="L22" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="M22" s="10" t="s">
+      <c r="M22" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="N22" s="10">
+      <c r="N22" s="21">
         <v>13</v>
       </c>
-      <c r="O22" s="10">
+      <c r="O22" s="21">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
-    </row>
-    <row r="23" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="18">
+      <c r="P22" s="22" t="s">
+        <v>452</v>
+      </c>
+      <c r="Q22" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="R22" s="22"/>
+    </row>
+    <row r="23" spans="1:18" s="23" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="19">
         <v>3</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="20">
         <v>44816.900532407402</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="H23" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="I23" s="10" t="s">
+      <c r="I23" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="J23" s="10" t="s">
+      <c r="J23" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="K23" s="10" t="s">
+      <c r="K23" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="L23" s="10" t="s">
+      <c r="L23" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="M23" s="10" t="s">
+      <c r="M23" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="N23" s="10">
+      <c r="N23" s="21">
         <v>3</v>
       </c>
-      <c r="O23" s="10">
+      <c r="O23" s="21">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-    </row>
-    <row r="24" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="18">
+      <c r="P23" s="22" t="s">
+        <v>452</v>
+      </c>
+      <c r="Q23" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="R23" s="22"/>
+    </row>
+    <row r="24" spans="1:18" s="23" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="19">
         <v>53</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="20" t="s">
         <v>446</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10">
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21">
         <v>53</v>
       </c>
-      <c r="O24" s="10">
+      <c r="O24" s="21">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-    </row>
-    <row r="25" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P24" s="22" t="s">
+        <v>452</v>
+      </c>
+      <c r="Q24" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="R24" s="22"/>
+    </row>
+    <row r="25" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <v>4</v>
       </c>
@@ -3886,7 +4009,7 @@
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
     </row>
-    <row r="27" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
         <v>44</v>
       </c>
@@ -3933,11 +4056,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="P27" s="8"/>
+      <c r="P27" s="8" t="s">
+        <v>453</v>
+      </c>
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
     </row>
-    <row r="28" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18">
         <v>34</v>
       </c>
@@ -3984,7 +4109,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="P28" s="8"/>
+      <c r="P28" s="8" t="s">
+        <v>453</v>
+      </c>
       <c r="Q28" s="8"/>
       <c r="R28" s="8"/>
     </row>
@@ -4041,7 +4168,7 @@
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
     </row>
-    <row r="30" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="18">
         <v>54</v>
       </c>
@@ -4066,11 +4193,13 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="P30" s="8"/>
+      <c r="P30" s="8" t="s">
+        <v>453</v>
+      </c>
       <c r="Q30" s="8"/>
       <c r="R30" s="8"/>
     </row>
-    <row r="31" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="18">
         <v>5</v>
       </c>
@@ -4123,7 +4252,7 @@
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
     </row>
-    <row r="32" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="18">
         <v>15</v>
       </c>
@@ -4170,11 +4299,13 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="P32" s="8"/>
+      <c r="P32" s="8" t="s">
+        <v>454</v>
+      </c>
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
     </row>
-    <row r="33" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="18">
         <v>25</v>
       </c>
@@ -4221,11 +4352,13 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="P33" s="8"/>
+      <c r="P33" s="8" t="s">
+        <v>454</v>
+      </c>
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
     </row>
-    <row r="34" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
         <v>45</v>
       </c>
@@ -4272,11 +4405,13 @@
         <f t="shared" ref="O34:O57" si="1">MOD(N34,10)</f>
         <v>5</v>
       </c>
-      <c r="P34" s="8"/>
+      <c r="P34" s="8" t="s">
+        <v>454</v>
+      </c>
       <c r="Q34" s="8"/>
       <c r="R34" s="8"/>
     </row>
-    <row r="35" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="18">
         <v>35</v>
       </c>
@@ -4323,11 +4458,13 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="P35" s="8"/>
+      <c r="P35" s="8" t="s">
+        <v>454</v>
+      </c>
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
     </row>
-    <row r="36" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="18">
         <v>55</v>
       </c>
@@ -4352,11 +4489,13 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="P36" s="8"/>
+      <c r="P36" s="8" t="s">
+        <v>454</v>
+      </c>
       <c r="Q36" s="8"/>
       <c r="R36" s="8"/>
     </row>
-    <row r="37" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="18">
         <v>46</v>
       </c>
@@ -4409,7 +4548,7 @@
       <c r="Q37" s="8"/>
       <c r="R37" s="8"/>
     </row>
-    <row r="38" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="18">
         <v>36</v>
       </c>
@@ -4456,11 +4595,13 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="P38" s="8"/>
+      <c r="P38" s="8" t="s">
+        <v>457</v>
+      </c>
       <c r="Q38" s="8"/>
       <c r="R38" s="8"/>
     </row>
-    <row r="39" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="18">
         <v>6</v>
       </c>
@@ -4507,11 +4648,13 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="P39" s="8"/>
+      <c r="P39" s="8" t="s">
+        <v>457</v>
+      </c>
       <c r="Q39" s="8"/>
       <c r="R39" s="8"/>
     </row>
-    <row r="40" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="18">
         <v>26</v>
       </c>
@@ -4558,11 +4701,13 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="P40" s="8"/>
+      <c r="P40" s="8" t="s">
+        <v>457</v>
+      </c>
       <c r="Q40" s="8"/>
       <c r="R40" s="8"/>
     </row>
-    <row r="41" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="18">
         <v>16</v>
       </c>
@@ -4607,11 +4752,13 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="P41" s="8"/>
+      <c r="P41" s="8" t="s">
+        <v>457</v>
+      </c>
       <c r="Q41" s="8"/>
       <c r="R41" s="8"/>
     </row>
-    <row r="42" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="18">
         <v>56</v>
       </c>
@@ -4636,11 +4783,13 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="P42" s="8"/>
+      <c r="P42" s="8" t="s">
+        <v>457</v>
+      </c>
       <c r="Q42" s="8"/>
       <c r="R42" s="8"/>
     </row>
-    <row r="43" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="18">
         <v>47</v>
       </c>
@@ -4693,7 +4842,7 @@
       <c r="Q43" s="8"/>
       <c r="R43" s="8"/>
     </row>
-    <row r="44" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="18">
         <v>17</v>
       </c>
@@ -4740,11 +4889,13 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="P44" s="8"/>
+      <c r="P44" s="8" t="s">
+        <v>456</v>
+      </c>
       <c r="Q44" s="8"/>
       <c r="R44" s="8"/>
     </row>
-    <row r="45" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="18">
         <v>27</v>
       </c>
@@ -4791,11 +4942,13 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="P45" s="8"/>
+      <c r="P45" s="8" t="s">
+        <v>456</v>
+      </c>
       <c r="Q45" s="8"/>
       <c r="R45" s="8"/>
     </row>
-    <row r="46" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="18">
         <v>7</v>
       </c>
@@ -4842,11 +4995,13 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="P46" s="8"/>
+      <c r="P46" s="8" t="s">
+        <v>456</v>
+      </c>
       <c r="Q46" s="8"/>
       <c r="R46" s="8"/>
     </row>
-    <row r="47" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="18">
         <v>37</v>
       </c>
@@ -4893,7 +5048,9 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="P47" s="8"/>
+      <c r="P47" s="8" t="s">
+        <v>456</v>
+      </c>
       <c r="Q47" s="8"/>
       <c r="R47" s="8"/>
     </row>
@@ -4947,7 +5104,9 @@
       <c r="P48" s="8" t="s">
         <v>458</v>
       </c>
-      <c r="Q48" s="8"/>
+      <c r="Q48" s="8" t="s">
+        <v>470</v>
+      </c>
       <c r="R48" s="8"/>
     </row>
     <row r="49" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5000,7 +5159,9 @@
       <c r="P49" s="8" t="s">
         <v>458</v>
       </c>
-      <c r="Q49" s="8"/>
+      <c r="Q49" s="8" t="s">
+        <v>470</v>
+      </c>
       <c r="R49" s="8"/>
     </row>
     <row r="50" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5106,7 +5267,9 @@
       <c r="P51" s="8" t="s">
         <v>458</v>
       </c>
-      <c r="Q51" s="8"/>
+      <c r="Q51" s="8" t="s">
+        <v>470</v>
+      </c>
       <c r="R51" s="8"/>
     </row>
     <row r="52" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -5159,10 +5322,12 @@
       <c r="P52" s="8" t="s">
         <v>458</v>
       </c>
-      <c r="Q52" s="8"/>
+      <c r="Q52" s="8" t="s">
+        <v>470</v>
+      </c>
       <c r="R52" s="8"/>
     </row>
-    <row r="53" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="18">
         <v>49</v>
       </c>
@@ -5215,7 +5380,7 @@
       <c r="Q53" s="8"/>
       <c r="R53" s="8"/>
     </row>
-    <row r="54" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="18">
         <v>19</v>
       </c>
@@ -5268,7 +5433,7 @@
       <c r="Q54" s="8"/>
       <c r="R54" s="8"/>
     </row>
-    <row r="55" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="18">
         <v>39</v>
       </c>
@@ -5321,7 +5486,7 @@
       <c r="Q55" s="8"/>
       <c r="R55" s="8"/>
     </row>
-    <row r="56" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="18">
         <v>9</v>
       </c>
@@ -5374,7 +5539,7 @@
       <c r="Q56" s="8"/>
       <c r="R56" s="8"/>
     </row>
-    <row r="57" spans="1:18" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="18">
         <v>29</v>
       </c>
@@ -7214,14 +7379,7 @@
       <c r="R151" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R57" xr:uid="{C3AB3A16-591D-B044-B64F-4E3FA8F26F09}">
-    <filterColumn colId="15">
-      <filters>
-        <filter val="Mono"/>
-        <filter val="Presentacion Menu Operaciones con mensajes"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:R57" xr:uid="{C3AB3A16-591D-B044-B64F-4E3FA8F26F09}"/>
   <sortState ref="A2:O57">
     <sortCondition ref="O2:O57"/>
     <sortCondition ref="D2:D57"/>

</xml_diff>

<commit_message>
Adicionando inser delete sqlite
</commit_message>
<xml_diff>
--- a/Nomina_trabajos finales.xlsx
+++ b/Nomina_trabajos finales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogerruizescobar/Documents/UDABOL/UDABOL_202202/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3ACFC9-92A5-6D47-87FB-63C869CCF138}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51FAF2A-BC77-B241-8C40-BE50F9844BBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="472">
   <si>
     <t>Leonardo</t>
   </si>
@@ -1442,6 +1442,9 @@
   </si>
   <si>
     <t>presentacion_mensaje</t>
+  </si>
+  <si>
+    <t>insertdelete_sqlite</t>
   </si>
 </sst>
 </file>
@@ -2628,8 +2631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L40" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q51" sqref="Q51:Q52"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="150" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2750,7 +2753,9 @@
       <c r="P2" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="Q2" s="8"/>
+      <c r="Q2" s="8" t="s">
+        <v>471</v>
+      </c>
       <c r="R2" s="8"/>
     </row>
     <row r="3" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2803,7 +2808,9 @@
       <c r="P3" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="Q3" s="8"/>
+      <c r="Q3" s="8" t="s">
+        <v>471</v>
+      </c>
       <c r="R3" s="8"/>
     </row>
     <row r="4" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2854,7 +2861,9 @@
       <c r="P4" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="Q4" s="8"/>
+      <c r="Q4" s="8" t="s">
+        <v>471</v>
+      </c>
       <c r="R4" s="8"/>
     </row>
     <row r="5" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2905,7 +2914,9 @@
       <c r="P5" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="Q5" s="8"/>
+      <c r="Q5" s="8" t="s">
+        <v>471</v>
+      </c>
       <c r="R5" s="8"/>
     </row>
     <row r="6" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2958,7 +2969,9 @@
       <c r="P6" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="Q6" s="8"/>
+      <c r="Q6" s="8" t="s">
+        <v>471</v>
+      </c>
       <c r="R6" s="8"/>
     </row>
     <row r="7" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3011,7 +3024,9 @@
       <c r="P7" s="8" t="s">
         <v>455</v>
       </c>
-      <c r="Q7" s="8"/>
+      <c r="Q7" s="8" t="s">
+        <v>471</v>
+      </c>
       <c r="R7" s="8"/>
     </row>
     <row r="8" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>